<commit_message>
Same as Last. Just updated Analysis code
</commit_message>
<xml_diff>
--- a/Modified Data Sets/COVID Cumulative Incidence (Through 2020-11-12) (ver2).xlsx
+++ b/Modified Data Sets/COVID Cumulative Incidence (Through 2020-11-12) (ver2).xlsx
@@ -2016,10 +2016,10 @@
         <v>12.9126213592233</v>
       </c>
       <c r="AP2">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ2">
-        <v>24.13574085836131</v>
+        <v>2.087169400736525</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -2147,10 +2147,10 @@
         <v>11.43145161290323</v>
       </c>
       <c r="AP3">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ3">
-        <v>21.36719927645463</v>
+        <v>1.847756187430478</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -2278,10 +2278,10 @@
         <v>12.3969465648855</v>
       </c>
       <c r="AP4">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ4">
-        <v>23.17186273810373</v>
+        <v>2.00381679389313</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -2381,14 +2381,35 @@
       <c r="AG5">
         <v>642.73</v>
       </c>
+      <c r="AH5">
+        <v>0.96875</v>
+      </c>
+      <c r="AI5">
+        <v>1.94140625</v>
+      </c>
+      <c r="AJ5">
+        <v>0.85546875</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>1.5</v>
+      </c>
+      <c r="AM5">
+        <v>1.109375</v>
+      </c>
+      <c r="AN5">
+        <v>0.90234375</v>
+      </c>
       <c r="AO5">
-        <v>0</v>
+        <v>7.27734375</v>
       </c>
       <c r="AP5">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>1.176294787176724</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -2516,10 +2537,10 @@
         <v>14.59307359307359</v>
       </c>
       <c r="AP6">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ6">
-        <v>27.2767730711656</v>
+        <v>2.358794223018361</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -2580,14 +2601,35 @@
       <c r="AG7">
         <v>382.89</v>
       </c>
+      <c r="AH7">
+        <v>1.454545454545455</v>
+      </c>
+      <c r="AI7">
+        <v>0.2987012987012987</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0.7337662337662337</v>
+      </c>
+      <c r="AL7">
+        <v>0.75</v>
+      </c>
+      <c r="AM7">
+        <v>0.461038961038961</v>
+      </c>
+      <c r="AN7">
+        <v>0.2142857142857143</v>
+      </c>
       <c r="AO7">
-        <v>0</v>
+        <v>3.912337662337662</v>
       </c>
       <c r="AP7">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>0.6323821652485446</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -2694,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="AP8">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ8">
         <v>0</v>
@@ -2825,10 +2867,10 @@
         <v>16.59227467811159</v>
       </c>
       <c r="AP9">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ9">
-        <v>31.01359752918054</v>
+        <v>2.681940950125796</v>
       </c>
     </row>
     <row r="10" spans="1:43">
@@ -2935,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ10">
         <v>0</v>
@@ -3026,14 +3068,35 @@
       <c r="AG11">
         <v>400.83</v>
       </c>
+      <c r="AH11">
+        <v>0.9707792207792207</v>
+      </c>
+      <c r="AI11">
+        <v>1.324675324675325</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0.7305194805194806</v>
+      </c>
+      <c r="AL11">
+        <v>1.844155844155844</v>
+      </c>
+      <c r="AM11">
+        <v>0.6753246753246753</v>
+      </c>
+      <c r="AN11">
+        <v>1.081168831168831</v>
+      </c>
       <c r="AO11">
-        <v>0</v>
+        <v>6.626623376623377</v>
       </c>
       <c r="AP11">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>1.071113692342141</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -3161,10 +3224,10 @@
         <v>9.578125</v>
       </c>
       <c r="AP12">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ12">
-        <v>17.90303738317757</v>
+        <v>1.548188308189655</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -3292,10 +3355,10 @@
         <v>8.16030534351145</v>
       </c>
       <c r="AP13">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ13">
-        <v>15.25290718413355</v>
+        <v>1.319014872334825</v>
       </c>
     </row>
     <row r="14" spans="1:43">
@@ -3423,10 +3486,10 @@
         <v>14.43968871595331</v>
       </c>
       <c r="AP14">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ14">
-        <v>26.99007236626787</v>
+        <v>2.33400140882866</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -3533,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="AP15">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ15">
         <v>0</v>
@@ -3664,10 +3727,10 @@
         <v>12.16346153846154</v>
       </c>
       <c r="AP16">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ16">
-        <v>22.73544212796549</v>
+        <v>1.96607675729443</v>
       </c>
     </row>
     <row r="17" spans="1:43">
@@ -3795,10 +3858,10 @@
         <v>14.72649572649573</v>
       </c>
       <c r="AP17">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ17">
-        <v>27.52616023644061</v>
+        <v>2.380360300618921</v>
       </c>
     </row>
     <row r="18" spans="1:43">
@@ -3901,14 +3964,35 @@
       <c r="AG18">
         <v>489.91</v>
       </c>
+      <c r="AH18">
+        <v>2.727272727272727</v>
+      </c>
+      <c r="AI18">
+        <v>1.5</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>1.5</v>
+      </c>
+      <c r="AL18">
+        <v>3.227272727272727</v>
+      </c>
+      <c r="AM18">
+        <v>2</v>
+      </c>
+      <c r="AN18">
+        <v>0.9545454545454546</v>
+      </c>
       <c r="AO18">
-        <v>0</v>
+        <v>11.90909090909091</v>
       </c>
       <c r="AP18">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ18">
-        <v>0</v>
+        <v>1.924960815047022</v>
       </c>
     </row>
     <row r="19" spans="1:43">
@@ -4036,10 +4120,10 @@
         <v>0.2239382239382239</v>
       </c>
       <c r="AP19">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ19">
-        <v>0.418576119510699</v>
+        <v>0.03619691119691119</v>
       </c>
     </row>
     <row r="20" spans="1:43">
@@ -4167,10 +4251,10 @@
         <v>9.614814814814814</v>
       </c>
       <c r="AP20">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ20">
-        <v>17.97161647628937</v>
+        <v>1.55411877394636</v>
       </c>
     </row>
     <row r="21" spans="1:43">
@@ -4298,10 +4382,10 @@
         <v>13.50877192982456</v>
       </c>
       <c r="AP21">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ21">
-        <v>25.25004099032628</v>
+        <v>2.183529945553539</v>
       </c>
     </row>
     <row r="22" spans="1:43">
@@ -4429,10 +4513,10 @@
         <v>10.38461538461538</v>
       </c>
       <c r="AP22">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ22">
-        <v>19.41049604601006</v>
+        <v>1.67854774535809</v>
       </c>
     </row>
     <row r="23" spans="1:43">
@@ -4526,14 +4610,35 @@
       <c r="AG23">
         <v>386.02</v>
       </c>
+      <c r="AH23">
+        <v>1.269480519480519</v>
+      </c>
+      <c r="AI23">
+        <v>1.136363636363636</v>
+      </c>
+      <c r="AJ23">
+        <v>0.4155844155844156</v>
+      </c>
+      <c r="AK23">
+        <v>0.5909090909090909</v>
+      </c>
+      <c r="AL23">
+        <v>2.227272727272727</v>
+      </c>
+      <c r="AM23">
+        <v>0.7694805194805194</v>
+      </c>
+      <c r="AN23">
+        <v>0.564935064935065</v>
+      </c>
       <c r="AO23">
-        <v>0</v>
+        <v>6.974025974025974</v>
       </c>
       <c r="AP23">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ23">
-        <v>0</v>
+        <v>1.127267129422302</v>
       </c>
     </row>
     <row r="24" spans="1:43">
@@ -4636,14 +4741,35 @@
       <c r="AG24">
         <v>433.21</v>
       </c>
+      <c r="AH24">
+        <v>2.657303370786517</v>
+      </c>
+      <c r="AI24">
+        <v>1.764044943820225</v>
+      </c>
+      <c r="AJ24">
+        <v>0.5393258426966292</v>
+      </c>
+      <c r="AK24">
+        <v>1.764044943820225</v>
+      </c>
+      <c r="AL24">
+        <v>3.421348314606742</v>
+      </c>
+      <c r="AM24">
+        <v>1.49438202247191</v>
+      </c>
+      <c r="AN24">
+        <v>0.8876404494382022</v>
+      </c>
       <c r="AO24">
-        <v>0</v>
+        <v>12.52808988764045</v>
       </c>
       <c r="AP24">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ24">
-        <v>0</v>
+        <v>2.025014529252228</v>
       </c>
     </row>
     <row r="25" spans="1:43">
@@ -4771,10 +4897,10 @@
         <v>17.11940298507463</v>
       </c>
       <c r="AP25">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ25">
-        <v>31.99888408425164</v>
+        <v>2.76714487905301</v>
       </c>
     </row>
     <row r="26" spans="1:43">
@@ -4902,10 +5028,10 @@
         <v>10.87449392712551</v>
       </c>
       <c r="AP26">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ26">
-        <v>20.32615687313179</v>
+        <v>1.757730699427614</v>
       </c>
     </row>
     <row r="27" spans="1:43">
@@ -5008,14 +5134,35 @@
       <c r="AG27">
         <v>455.4</v>
       </c>
+      <c r="AH27">
+        <v>1.890350877192982</v>
+      </c>
+      <c r="AI27">
+        <v>1.315789473684211</v>
+      </c>
+      <c r="AJ27">
+        <v>0.2675438596491228</v>
+      </c>
+      <c r="AK27">
+        <v>1.732456140350877</v>
+      </c>
+      <c r="AL27">
+        <v>3.258771929824561</v>
+      </c>
+      <c r="AM27">
+        <v>1.491228070175439</v>
+      </c>
+      <c r="AN27">
+        <v>1.219298245614035</v>
+      </c>
       <c r="AO27">
-        <v>0</v>
+        <v>11.17543859649123</v>
       </c>
       <c r="AP27">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ27">
-        <v>0</v>
+        <v>1.806374773139746</v>
       </c>
     </row>
     <row r="28" spans="1:43">
@@ -5143,10 +5290,10 @@
         <v>15.10322580645161</v>
       </c>
       <c r="AP28">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ28">
-        <v>28.23032861018993</v>
+        <v>2.441254171301446</v>
       </c>
     </row>
     <row r="29" spans="1:43">
@@ -5225,14 +5372,35 @@
       <c r="AG29">
         <v>401.62</v>
       </c>
+      <c r="AH29">
+        <v>1.626623376623377</v>
+      </c>
+      <c r="AI29">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <v>0.07792207792207792</v>
+      </c>
+      <c r="AL29">
+        <v>1.75</v>
+      </c>
+      <c r="AM29">
+        <v>1.103896103896104</v>
+      </c>
+      <c r="AN29">
+        <v>1.146103896103896</v>
+      </c>
       <c r="AO29">
-        <v>0</v>
+        <v>6.613636363636363</v>
       </c>
       <c r="AP29">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ29">
-        <v>0</v>
+        <v>1.069014498432602</v>
       </c>
     </row>
     <row r="30" spans="1:43">
@@ -5360,10 +5528,10 @@
         <v>5.636363636363636</v>
       </c>
       <c r="AP30">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ30">
-        <v>10.53525913338997</v>
+        <v>0.9110501567398118</v>
       </c>
     </row>
     <row r="31" spans="1:43">
@@ -5491,10 +5659,10 @@
         <v>7.322580645161291</v>
       </c>
       <c r="AP31">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ31">
-        <v>13.6870666264697</v>
+        <v>1.183606785317019</v>
       </c>
     </row>
     <row r="32" spans="1:43">
@@ -5622,10 +5790,10 @@
         <v>8.695876288659793</v>
       </c>
       <c r="AP32">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ32">
-        <v>16.25397437132672</v>
+        <v>1.405583451830785</v>
       </c>
     </row>
     <row r="33" spans="1:43">
@@ -5690,7 +5858,7 @@
         <v>0</v>
       </c>
       <c r="AP33">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ33">
         <v>0</v>
@@ -5796,11 +5964,32 @@
       <c r="AG34">
         <v>438.44</v>
       </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <v>0</v>
+      </c>
+      <c r="AN34">
+        <v>0</v>
+      </c>
       <c r="AO34">
         <v>0</v>
       </c>
       <c r="AP34">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ34">
         <v>0</v>
@@ -5931,10 +6120,10 @@
         <v>13.67464114832536</v>
       </c>
       <c r="AP35">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ35">
-        <v>25.56007691275768</v>
+        <v>2.210340702854314</v>
       </c>
     </row>
     <row r="36" spans="1:43">
@@ -6062,10 +6251,10 @@
         <v>2.228070175438596</v>
       </c>
       <c r="AP36">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ36">
-        <v>4.164617150352516</v>
+        <v>0.3601406533575318</v>
       </c>
     </row>
     <row r="37" spans="1:43">
@@ -6193,10 +6382,10 @@
         <v>9.50925925925926</v>
       </c>
       <c r="AP37">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ37">
-        <v>17.77431637244721</v>
+        <v>1.537056992337165</v>
       </c>
     </row>
     <row r="38" spans="1:43">
@@ -6324,10 +6513,10 @@
         <v>11.05821917808219</v>
       </c>
       <c r="AP38">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ38">
-        <v>20.66956855716298</v>
+        <v>1.787427668871044</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -6412,14 +6601,35 @@
       <c r="AG39">
         <v>461.06</v>
       </c>
+      <c r="AH39">
+        <v>1.051948051948052</v>
+      </c>
+      <c r="AI39">
+        <v>0.8701298701298701</v>
+      </c>
+      <c r="AJ39">
+        <v>0.538961038961039</v>
+      </c>
+      <c r="AK39">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="AL39">
+        <v>1.564935064935065</v>
+      </c>
+      <c r="AM39">
+        <v>0.961038961038961</v>
+      </c>
+      <c r="AN39">
+        <v>0.6558441558441559</v>
+      </c>
       <c r="AO39">
-        <v>0</v>
+        <v>6.285714285714285</v>
       </c>
       <c r="AP39">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ39">
-        <v>0</v>
+        <v>1.016009852216749</v>
       </c>
     </row>
     <row r="40" spans="1:43">
@@ -6522,14 +6732,35 @@
       <c r="AG40">
         <v>336.93</v>
       </c>
+      <c r="AH40">
+        <v>2.616279069767442</v>
+      </c>
+      <c r="AI40">
+        <v>1.744186046511628</v>
+      </c>
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+      <c r="AK40">
+        <v>1.744186046511628</v>
+      </c>
+      <c r="AL40">
+        <v>2.616279069767442</v>
+      </c>
+      <c r="AM40">
+        <v>1.744186046511628</v>
+      </c>
+      <c r="AN40">
+        <v>0.7441860465116279</v>
+      </c>
       <c r="AO40">
-        <v>0</v>
+        <v>11.20930232558139</v>
       </c>
       <c r="AP40">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ40">
-        <v>0</v>
+        <v>1.811848436246993</v>
       </c>
     </row>
     <row r="41" spans="1:43">
@@ -6632,14 +6863,35 @@
       <c r="AG41">
         <v>362.25</v>
       </c>
+      <c r="AH41">
+        <v>1.744769874476988</v>
+      </c>
+      <c r="AI41">
+        <v>1.774058577405858</v>
+      </c>
+      <c r="AJ41">
+        <v>0.4811715481171548</v>
+      </c>
+      <c r="AK41">
+        <v>1.560669456066946</v>
+      </c>
+      <c r="AL41">
+        <v>3.05020920502092</v>
+      </c>
+      <c r="AM41">
+        <v>1.698744769874477</v>
+      </c>
+      <c r="AN41">
+        <v>1.790794979079498</v>
+      </c>
       <c r="AO41">
-        <v>0</v>
+        <v>12.10041841004184</v>
       </c>
       <c r="AP41">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ41">
-        <v>0</v>
+        <v>1.955886596450729</v>
       </c>
     </row>
     <row r="42" spans="1:43">
@@ -6767,10 +7019,10 @@
         <v>11.67567567567568</v>
       </c>
       <c r="AP42">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ42">
-        <v>21.82369285173024</v>
+        <v>1.887232059645853</v>
       </c>
     </row>
     <row r="43" spans="1:43">
@@ -6898,10 +7150,10 @@
         <v>17.69565217391304</v>
       </c>
       <c r="AP43">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ43">
-        <v>33.07598537180008</v>
+        <v>2.860288605697151</v>
       </c>
     </row>
     <row r="44" spans="1:43">
@@ -7029,10 +7281,10 @@
         <v>15.0609756097561</v>
       </c>
       <c r="AP44">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ44">
-        <v>28.15135627991794</v>
+        <v>2.434424936921783</v>
       </c>
     </row>
     <row r="45" spans="1:43">
@@ -7139,7 +7391,7 @@
         <v>0</v>
       </c>
       <c r="AP45">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ45">
         <v>0</v>
@@ -7179,14 +7431,35 @@
       <c r="U46">
         <v>0</v>
       </c>
+      <c r="AH46">
+        <v>1.516233766233766</v>
+      </c>
+      <c r="AI46">
+        <v>1.743506493506493</v>
+      </c>
+      <c r="AJ46">
+        <v>0.5681818181818182</v>
+      </c>
+      <c r="AK46">
+        <v>0.7467532467532467</v>
+      </c>
+      <c r="AL46">
+        <v>2.025974025974026</v>
+      </c>
+      <c r="AM46">
+        <v>1.305194805194805</v>
+      </c>
+      <c r="AN46">
+        <v>1.516233766233766</v>
+      </c>
       <c r="AO46">
-        <v>0</v>
+        <v>9.422077922077921</v>
       </c>
       <c r="AP46">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ46">
-        <v>0</v>
+        <v>1.522965181370354</v>
       </c>
     </row>
     <row r="47" spans="1:43">
@@ -7227,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="AP47">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ47">
         <v>0</v>
@@ -7271,7 +7544,7 @@
         <v>0</v>
       </c>
       <c r="AP48">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ48">
         <v>0</v>
@@ -7402,10 +7675,10 @@
         <v>11.64532019704433</v>
       </c>
       <c r="AP49">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ49">
-        <v>21.76695363933521</v>
+        <v>1.882325462884321</v>
       </c>
     </row>
     <row r="50" spans="1:43">
@@ -7533,10 +7806,10 @@
         <v>11.56862745098039</v>
       </c>
       <c r="AP50">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ50">
-        <v>21.62360271211288</v>
+        <v>1.869929006085193</v>
       </c>
     </row>
     <row r="51" spans="1:43">
@@ -7664,10 +7937,10 @@
         <v>6.782442748091603</v>
       </c>
       <c r="AP51">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ51">
-        <v>12.67746308054505</v>
+        <v>1.096300013161358</v>
       </c>
     </row>
     <row r="52" spans="1:43">
@@ -7795,10 +8068,10 @@
         <v>13.45</v>
       </c>
       <c r="AP52">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ52">
-        <v>25.14018691588785</v>
+        <v>2.174030172413793</v>
       </c>
     </row>
     <row r="53" spans="1:43">
@@ -7926,10 +8199,10 @@
         <v>10.77459016393443</v>
       </c>
       <c r="AP53">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ53">
-        <v>20.13942086716715</v>
+        <v>1.741582461842849</v>
       </c>
     </row>
     <row r="54" spans="1:43">
@@ -8008,14 +8281,35 @@
       <c r="Y54">
         <v>246489</v>
       </c>
+      <c r="AH54">
+        <v>1.301948051948052</v>
+      </c>
+      <c r="AI54">
+        <v>1.126623376623377</v>
+      </c>
+      <c r="AJ54">
+        <v>0</v>
+      </c>
+      <c r="AK54">
+        <v>0.525974025974026</v>
+      </c>
+      <c r="AL54">
+        <v>1.808441558441559</v>
+      </c>
+      <c r="AM54">
+        <v>0.9967532467532467</v>
+      </c>
+      <c r="AN54">
+        <v>0.4188311688311688</v>
+      </c>
       <c r="AO54">
-        <v>0</v>
+        <v>6.178571428571429</v>
       </c>
       <c r="AP54">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ54">
-        <v>0</v>
+        <v>0.9986915024630543</v>
       </c>
     </row>
     <row r="55" spans="1:43">
@@ -8080,7 +8374,7 @@
         <v>0</v>
       </c>
       <c r="AP55">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ55">
         <v>0</v>
@@ -8186,14 +8480,35 @@
       <c r="AG56">
         <v>360.87</v>
       </c>
+      <c r="AH56">
+        <v>1.402597402597403</v>
+      </c>
+      <c r="AI56">
+        <v>1.331168831168831</v>
+      </c>
+      <c r="AJ56">
+        <v>1.159090909090909</v>
+      </c>
+      <c r="AK56">
+        <v>1.448051948051948</v>
+      </c>
+      <c r="AL56">
+        <v>1.168831168831169</v>
+      </c>
+      <c r="AM56">
+        <v>1.126623376623377</v>
+      </c>
+      <c r="AN56">
+        <v>1.00974025974026</v>
+      </c>
       <c r="AO56">
-        <v>0</v>
+        <v>8.646103896103897</v>
       </c>
       <c r="AP56">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ56">
-        <v>0</v>
+        <v>1.397538345275414</v>
       </c>
     </row>
     <row r="57" spans="1:43">
@@ -8296,14 +8611,35 @@
       <c r="AG57">
         <v>350.11</v>
       </c>
+      <c r="AH57">
+        <v>1.402597402597403</v>
+      </c>
+      <c r="AI57">
+        <v>1.331168831168831</v>
+      </c>
+      <c r="AJ57">
+        <v>1.159090909090909</v>
+      </c>
+      <c r="AK57">
+        <v>1.448051948051948</v>
+      </c>
+      <c r="AL57">
+        <v>1.168831168831169</v>
+      </c>
+      <c r="AM57">
+        <v>1.126623376623377</v>
+      </c>
+      <c r="AN57">
+        <v>1.00974025974026</v>
+      </c>
       <c r="AO57">
-        <v>0</v>
+        <v>8.646103896103897</v>
       </c>
       <c r="AP57">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ57">
-        <v>0</v>
+        <v>1.397538345275414</v>
       </c>
     </row>
     <row r="58" spans="1:43">
@@ -8431,10 +8767,10 @@
         <v>8.885826771653543</v>
       </c>
       <c r="AP58">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ58">
-        <v>16.60902200309073</v>
+        <v>1.436286654900896</v>
       </c>
     </row>
     <row r="59" spans="1:43">
@@ -8475,7 +8811,7 @@
         <v>0</v>
       </c>
       <c r="AP59">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ59">
         <v>0</v>
@@ -8606,10 +8942,10 @@
         <v>15.84415584415584</v>
       </c>
       <c r="AP60">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ60">
-        <v>29.61524456851559</v>
+        <v>2.561016569637259</v>
       </c>
     </row>
     <row r="61" spans="1:43">
@@ -8734,10 +9070,10 @@
         <v>7.960698689956331</v>
       </c>
       <c r="AP61">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ61">
-        <v>14.87981063543239</v>
+        <v>1.286750865833459</v>
       </c>
     </row>
     <row r="62" spans="1:43">
@@ -8865,10 +9201,10 @@
         <v>13.56862745098039</v>
       </c>
       <c r="AP62">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ62">
-        <v>25.36192046912223</v>
+        <v>2.193204868154158</v>
       </c>
     </row>
     <row r="63" spans="1:43">
@@ -8996,10 +9332,10 @@
         <v>12.49090909090909</v>
       </c>
       <c r="AP63">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ63">
-        <v>23.34749362786746</v>
+        <v>2.019004702194358</v>
       </c>
     </row>
     <row r="64" spans="1:43">
@@ -9127,10 +9463,10 @@
         <v>9.693548387096774</v>
       </c>
       <c r="AP64">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ64">
-        <v>18.11878203195659</v>
+        <v>1.56684510567297</v>
       </c>
     </row>
     <row r="65" spans="1:43">
@@ -9258,10 +9594,10 @@
         <v>17.37241379310345</v>
       </c>
       <c r="AP65">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ65">
-        <v>32.47180148243635</v>
+        <v>2.808041022592152</v>
       </c>
     </row>
     <row r="66" spans="1:43">
@@ -9368,7 +9704,7 @@
         <v>0</v>
       </c>
       <c r="AP66">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ66">
         <v>0</v>
@@ -9465,14 +9801,35 @@
       <c r="AG67">
         <v>440.32</v>
       </c>
+      <c r="AH67">
+        <v>2.8</v>
+      </c>
+      <c r="AI67">
+        <v>2.655555555555555</v>
+      </c>
+      <c r="AJ67">
+        <v>1.911111111111111</v>
+      </c>
+      <c r="AK67">
+        <v>1.933333333333333</v>
+      </c>
+      <c r="AL67">
+        <v>3.911111111111111</v>
+      </c>
+      <c r="AM67">
+        <v>1.955555555555555</v>
+      </c>
+      <c r="AN67">
+        <v>1.855555555555556</v>
+      </c>
       <c r="AO67">
-        <v>0</v>
+        <v>17.02222222222222</v>
       </c>
       <c r="AP67">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ67">
-        <v>0</v>
+        <v>2.751436781609196</v>
       </c>
     </row>
     <row r="68" spans="1:43">
@@ -9600,10 +9957,10 @@
         <v>5.146153846153847</v>
       </c>
       <c r="AP68">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ68">
-        <v>9.618979151689432</v>
+        <v>0.8318136604774536</v>
       </c>
     </row>
     <row r="69" spans="1:43">
@@ -9731,10 +10088,10 @@
         <v>14.17532467532468</v>
       </c>
       <c r="AP69">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ69">
-        <v>26.49593397256949</v>
+        <v>2.291270152261532</v>
       </c>
     </row>
     <row r="70" spans="1:43">
@@ -9862,10 +10219,10 @@
         <v>14.7125748502994</v>
       </c>
       <c r="AP70">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ70">
-        <v>27.50013990710168</v>
+        <v>2.37811015899236</v>
       </c>
     </row>
     <row r="71" spans="1:43">
@@ -9902,14 +10259,35 @@
       <c r="U71">
         <v>0</v>
       </c>
+      <c r="AH71">
+        <v>0.448051948051948</v>
+      </c>
+      <c r="AI71">
+        <v>0.6201298701298701</v>
+      </c>
+      <c r="AJ71">
+        <v>0</v>
+      </c>
+      <c r="AK71">
+        <v>0.474025974025974</v>
+      </c>
+      <c r="AL71">
+        <v>1.214285714285714</v>
+      </c>
+      <c r="AM71">
+        <v>0.5324675324675324</v>
+      </c>
+      <c r="AN71">
+        <v>0.2987012987012987</v>
+      </c>
       <c r="AO71">
-        <v>0</v>
+        <v>3.587662337662338</v>
       </c>
       <c r="AP71">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ71">
-        <v>0</v>
+        <v>0.5799023175100761</v>
       </c>
     </row>
     <row r="72" spans="1:43">
@@ -10012,14 +10390,35 @@
       <c r="AG72">
         <v>462.38</v>
       </c>
+      <c r="AH72">
+        <v>3</v>
+      </c>
+      <c r="AI72">
+        <v>3</v>
+      </c>
+      <c r="AJ72">
+        <v>2</v>
+      </c>
+      <c r="AK72">
+        <v>2</v>
+      </c>
+      <c r="AL72">
+        <v>3</v>
+      </c>
+      <c r="AM72">
+        <v>2.3</v>
+      </c>
+      <c r="AN72">
+        <v>2</v>
+      </c>
       <c r="AO72">
-        <v>0</v>
+        <v>17.3</v>
       </c>
       <c r="AP72">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ72">
-        <v>0</v>
+        <v>2.796336206896552</v>
       </c>
     </row>
     <row r="73" spans="1:43">
@@ -10147,10 +10546,10 @@
         <v>5</v>
       </c>
       <c r="AP73">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ73">
-        <v>9.345794392523365</v>
+        <v>0.8081896551724138</v>
       </c>
     </row>
     <row r="74" spans="1:43">
@@ -10278,10 +10677,10 @@
         <v>9.241379310344827</v>
       </c>
       <c r="AP74">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ74">
-        <v>17.27360618756042</v>
+        <v>1.493757431629013</v>
       </c>
     </row>
     <row r="75" spans="1:43">
@@ -10384,14 +10783,35 @@
       <c r="AG75">
         <v>452.63</v>
       </c>
+      <c r="AH75">
+        <v>1.282786885245902</v>
+      </c>
+      <c r="AI75">
+        <v>1.864754098360656</v>
+      </c>
+      <c r="AJ75">
+        <v>0.860655737704918</v>
+      </c>
+      <c r="AK75">
+        <v>1.631147540983606</v>
+      </c>
+      <c r="AL75">
+        <v>3.692622950819672</v>
+      </c>
+      <c r="AM75">
+        <v>1.860655737704918</v>
+      </c>
+      <c r="AN75">
+        <v>1.065573770491803</v>
+      </c>
       <c r="AO75">
-        <v>0</v>
+        <v>12.25819672131147</v>
       </c>
       <c r="AP75">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ75">
-        <v>0</v>
+        <v>1.981389556246467</v>
       </c>
     </row>
     <row r="76" spans="1:43">
@@ -10519,10 +10939,10 @@
         <v>12.3375796178344</v>
       </c>
       <c r="AP76">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ76">
-        <v>23.06089648193345</v>
+        <v>1.994220843399956</v>
       </c>
     </row>
     <row r="77" spans="1:43">
@@ -10650,10 +11070,10 @@
         <v>11.82758620689655</v>
       </c>
       <c r="AP77">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ77">
-        <v>22.1076377699001</v>
+        <v>1.911786563614744</v>
       </c>
     </row>
     <row r="78" spans="1:43">
@@ -10781,10 +11201,10 @@
         <v>9.349480968858131</v>
       </c>
       <c r="AP78">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ78">
-        <v>17.47566536235165</v>
+        <v>1.5112307600525</v>
       </c>
     </row>
     <row r="79" spans="1:43">
@@ -10887,14 +11307,35 @@
       <c r="AG79">
         <v>449.78</v>
       </c>
+      <c r="AH79">
+        <v>2.681159420289855</v>
+      </c>
+      <c r="AI79">
+        <v>1.188405797101449</v>
+      </c>
+      <c r="AJ79">
+        <v>0.5652173913043478</v>
+      </c>
+      <c r="AK79">
+        <v>0.2898550724637681</v>
+      </c>
+      <c r="AL79">
+        <v>2.956521739130435</v>
+      </c>
+      <c r="AM79">
+        <v>1.971014492753623</v>
+      </c>
+      <c r="AN79">
+        <v>0.2898550724637681</v>
+      </c>
       <c r="AO79">
-        <v>0</v>
+        <v>9.942028985507246</v>
       </c>
       <c r="AP79">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ79">
-        <v>0</v>
+        <v>1.607008995502249</v>
       </c>
     </row>
     <row r="80" spans="1:43">
@@ -10970,14 +11411,35 @@
       <c r="AG80">
         <v>469.78</v>
       </c>
+      <c r="AH80">
+        <v>1.314935064935065</v>
+      </c>
+      <c r="AI80">
+        <v>1.016233766233766</v>
+      </c>
+      <c r="AJ80">
+        <v>0.5194805194805194</v>
+      </c>
+      <c r="AK80">
+        <v>0</v>
+      </c>
+      <c r="AL80">
+        <v>1.873376623376623</v>
+      </c>
+      <c r="AM80">
+        <v>1.097402597402597</v>
+      </c>
+      <c r="AN80">
+        <v>0.4285714285714285</v>
+      </c>
       <c r="AO80">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="AP80">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ80">
-        <v>0</v>
+        <v>1.010237068965517</v>
       </c>
     </row>
     <row r="81" spans="1:43">
@@ -11105,10 +11567,10 @@
         <v>9.942528735632184</v>
       </c>
       <c r="AP81">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ81">
-        <v>18.58416586099474</v>
+        <v>1.607089774078478</v>
       </c>
     </row>
     <row r="82" spans="1:43">
@@ -11208,14 +11670,35 @@
       <c r="AG82">
         <v>513.4400000000001</v>
       </c>
+      <c r="AH82">
+        <v>1.061688311688312</v>
+      </c>
+      <c r="AI82">
+        <v>0.2597402597402597</v>
+      </c>
+      <c r="AJ82">
+        <v>0.1558441558441558</v>
+      </c>
+      <c r="AK82">
+        <v>0.8798701298701299</v>
+      </c>
+      <c r="AL82">
+        <v>1.616883116883117</v>
+      </c>
+      <c r="AM82">
+        <v>1.048701298701299</v>
+      </c>
+      <c r="AN82">
+        <v>0.288961038961039</v>
+      </c>
       <c r="AO82">
-        <v>0</v>
+        <v>5.311688311688313</v>
       </c>
       <c r="AP82">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ82">
-        <v>0</v>
+        <v>0.8585703090013437</v>
       </c>
     </row>
     <row r="83" spans="1:43">
@@ -11322,7 +11805,7 @@
         <v>0</v>
       </c>
       <c r="AP83">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ83">
         <v>0</v>
@@ -11428,14 +11911,35 @@
       <c r="AG84">
         <v>411.29</v>
       </c>
+      <c r="AH84">
+        <v>2.220779220779221</v>
+      </c>
+      <c r="AI84">
+        <v>1.701298701298701</v>
+      </c>
+      <c r="AJ84">
+        <v>0.5487012987012987</v>
+      </c>
+      <c r="AK84">
+        <v>0.2467532467532468</v>
+      </c>
+      <c r="AL84">
+        <v>2.691558441558441</v>
+      </c>
+      <c r="AM84">
+        <v>1.467532467532467</v>
+      </c>
+      <c r="AN84">
+        <v>0.8733766233766234</v>
+      </c>
       <c r="AO84">
-        <v>0</v>
+        <v>9.750000000000002</v>
       </c>
       <c r="AP84">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ84">
-        <v>0</v>
+        <v>1.575969827586207</v>
       </c>
     </row>
     <row r="85" spans="1:43">
@@ -11563,10 +12067,10 @@
         <v>17.77443609022556</v>
       </c>
       <c r="AP85">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ85">
-        <v>33.223245028459</v>
+        <v>2.873023074928701</v>
       </c>
     </row>
     <row r="86" spans="1:43">
@@ -11694,10 +12198,10 @@
         <v>12.30188679245283</v>
       </c>
       <c r="AP86">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ86">
-        <v>22.99418092047258</v>
+        <v>1.988451528952505</v>
       </c>
     </row>
     <row r="87" spans="1:43">
@@ -11804,7 +12308,7 @@
         <v>0</v>
       </c>
       <c r="AP87">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ87">
         <v>0</v>
@@ -11935,10 +12439,10 @@
         <v>13.6969696969697</v>
       </c>
       <c r="AP88">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ88">
-        <v>25.60181251770037</v>
+        <v>2.213949843260188</v>
       </c>
     </row>
     <row r="89" spans="1:43">
@@ -12066,10 +12570,10 @@
         <v>16.86585365853659</v>
       </c>
       <c r="AP89">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ89">
-        <v>31.52496010941418</v>
+        <v>2.726161690496216</v>
       </c>
     </row>
     <row r="90" spans="1:43">
@@ -12110,7 +12614,7 @@
         <v>0</v>
       </c>
       <c r="AP90">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ90">
         <v>0</v>
@@ -12241,10 +12745,10 @@
         <v>18.03759398496241</v>
       </c>
       <c r="AP91">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ91">
-        <v>33.71512894385496</v>
+        <v>2.915559372569354</v>
       </c>
     </row>
     <row r="92" spans="1:43">
@@ -12332,14 +12836,35 @@
       <c r="AG92">
         <v>690.54</v>
       </c>
+      <c r="AH92">
+        <v>2.350649350649351</v>
+      </c>
+      <c r="AI92">
+        <v>1.25</v>
+      </c>
+      <c r="AJ92">
+        <v>0</v>
+      </c>
+      <c r="AK92">
+        <v>0</v>
+      </c>
+      <c r="AL92">
+        <v>2.623376623376624</v>
+      </c>
+      <c r="AM92">
+        <v>1.662337662337662</v>
+      </c>
+      <c r="AN92">
+        <v>0.7012987012987013</v>
+      </c>
       <c r="AO92">
-        <v>0</v>
+        <v>8.587662337662337</v>
       </c>
       <c r="AP92">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ92">
-        <v>0</v>
+        <v>1.38809197268249</v>
       </c>
     </row>
     <row r="93" spans="1:43">
@@ -12467,10 +12992,10 @@
         <v>8.170634920634921</v>
       </c>
       <c r="AP93">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ93">
-        <v>15.27221480492509</v>
+        <v>1.320684523809524</v>
       </c>
     </row>
     <row r="94" spans="1:43">
@@ -12598,10 +13123,10 @@
         <v>6.145374449339208</v>
       </c>
       <c r="AP94">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ94">
-        <v>11.48668121371815</v>
+        <v>0.9933256114233634</v>
       </c>
     </row>
     <row r="95" spans="1:43">
@@ -12729,10 +13254,10 @@
         <v>13.45454545454545</v>
       </c>
       <c r="AP95">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ95">
-        <v>25.14868309260832</v>
+        <v>2.174764890282132</v>
       </c>
     </row>
     <row r="96" spans="1:43">
@@ -12860,10 +13385,10 @@
         <v>13.32057416267943</v>
       </c>
       <c r="AP96">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ96">
-        <v>24.8982694629522</v>
+        <v>2.15311004784689</v>
       </c>
     </row>
     <row r="97" spans="1:43">
@@ -12991,10 +13516,10 @@
         <v>10.11194029850746</v>
       </c>
       <c r="AP97">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ97">
-        <v>18.90082298786442</v>
+        <v>1.634473108594956</v>
       </c>
     </row>
     <row r="98" spans="1:43">
@@ -13122,10 +13647,10 @@
         <v>16.19597989949749</v>
       </c>
       <c r="AP98">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ98">
-        <v>30.27285962522895</v>
+        <v>2.617884682030844</v>
       </c>
     </row>
     <row r="99" spans="1:43">
@@ -13253,10 +13778,10 @@
         <v>12.45762711864407</v>
       </c>
       <c r="AP99">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ99">
-        <v>23.28528433391415</v>
+        <v>2.013625073056692</v>
       </c>
     </row>
     <row r="100" spans="1:43">
@@ -13384,10 +13909,10 @@
         <v>10.80630630630631</v>
       </c>
       <c r="AP100">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ100">
-        <v>20.19870337627347</v>
+        <v>1.746708993476235</v>
       </c>
     </row>
     <row r="101" spans="1:43">
@@ -13515,10 +14040,10 @@
         <v>9.763066202090592</v>
       </c>
       <c r="AP101">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ101">
-        <v>18.24872187306653</v>
+        <v>1.578081821458609</v>
       </c>
     </row>
     <row r="102" spans="1:43">
@@ -13646,10 +14171,10 @@
         <v>13.83756345177665</v>
       </c>
       <c r="AP102">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ102">
-        <v>25.86460458276009</v>
+        <v>2.236675126903553</v>
       </c>
     </row>
     <row r="103" spans="1:43">
@@ -13777,10 +14302,10 @@
         <v>4.162436548223351</v>
       </c>
       <c r="AP103">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ103">
-        <v>7.78025523032402</v>
+        <v>0.6728076317171364</v>
       </c>
     </row>
     <row r="104" spans="1:43">
@@ -13908,10 +14433,10 @@
         <v>10.98039215686275</v>
       </c>
       <c r="AP104">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ104">
-        <v>20.52409748946307</v>
+        <v>1.774847870182556</v>
       </c>
     </row>
     <row r="105" spans="1:43">
@@ -14039,10 +14564,10 @@
         <v>16.88888888888889</v>
       </c>
       <c r="AP105">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ105">
-        <v>31.56801661474559</v>
+        <v>2.729885057471265</v>
       </c>
     </row>
     <row r="106" spans="1:43">
@@ -14170,10 +14695,10 @@
         <v>13.88477366255144</v>
       </c>
       <c r="AP106">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ106">
-        <v>25.95284796738587</v>
+        <v>2.244306087696892</v>
       </c>
     </row>
     <row r="107" spans="1:43">
@@ -14268,10 +14793,10 @@
         <v>13.25819672131148</v>
       </c>
       <c r="AP107">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ107">
-        <v>24.78167611460089</v>
+        <v>2.14302748728095</v>
       </c>
     </row>
     <row r="108" spans="1:43">
@@ -14399,10 +14924,10 @@
         <v>14.1123595505618</v>
       </c>
       <c r="AP108">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ108">
-        <v>26.3782421505828</v>
+        <v>2.281092599767532</v>
       </c>
     </row>
     <row r="109" spans="1:43">
@@ -14481,14 +15006,35 @@
       <c r="Y109">
         <v>8455</v>
       </c>
+      <c r="AH109">
+        <v>2.048701298701299</v>
+      </c>
+      <c r="AI109">
+        <v>1.61038961038961</v>
+      </c>
+      <c r="AJ109">
+        <v>1.175324675324675</v>
+      </c>
+      <c r="AK109">
+        <v>1.399350649350649</v>
+      </c>
+      <c r="AL109">
+        <v>2.961038961038961</v>
+      </c>
+      <c r="AM109">
+        <v>1.571428571428571</v>
+      </c>
+      <c r="AN109">
+        <v>1.477272727272727</v>
+      </c>
       <c r="AO109">
-        <v>0</v>
+        <v>12.24350649350649</v>
       </c>
       <c r="AP109">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ109">
-        <v>0</v>
+        <v>1.979015058217644</v>
       </c>
     </row>
     <row r="110" spans="1:43">
@@ -14553,7 +15099,7 @@
         <v>0</v>
       </c>
       <c r="AP110">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ110">
         <v>0</v>
@@ -14659,14 +15205,35 @@
       <c r="AG111">
         <v>447.91</v>
       </c>
+      <c r="AH111">
+        <v>1</v>
+      </c>
+      <c r="AI111">
+        <v>1.572649572649573</v>
+      </c>
+      <c r="AJ111">
+        <v>0.4188034188034188</v>
+      </c>
+      <c r="AK111">
+        <v>0.4188034188034188</v>
+      </c>
+      <c r="AL111">
+        <v>1.273504273504273</v>
+      </c>
+      <c r="AM111">
+        <v>1.286324786324786</v>
+      </c>
+      <c r="AN111">
+        <v>0.2991452991452991</v>
+      </c>
       <c r="AO111">
-        <v>0</v>
+        <v>6.269230769230768</v>
       </c>
       <c r="AP111">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ111">
-        <v>0</v>
+        <v>1.01334549071618</v>
       </c>
     </row>
     <row r="112" spans="1:43">
@@ -14794,10 +15361,10 @@
         <v>7.34375</v>
       </c>
       <c r="AP112">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ112">
-        <v>13.72663551401869</v>
+        <v>1.187028556034483</v>
       </c>
     </row>
     <row r="113" spans="1:43">
@@ -14925,10 +15492,10 @@
         <v>10.68965517241379</v>
       </c>
       <c r="AP113">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ113">
-        <v>19.98066387367064</v>
+        <v>1.727853745541023</v>
       </c>
     </row>
     <row r="114" spans="1:43">
@@ -15056,10 +15623,10 @@
         <v>20.58024691358025</v>
       </c>
       <c r="AP114">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ114">
-        <v>38.46775124033691</v>
+        <v>3.326548531289911</v>
       </c>
     </row>
     <row r="115" spans="1:43">
@@ -15187,10 +15754,10 @@
         <v>15.68367346938776</v>
       </c>
       <c r="AP115">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ115">
-        <v>29.31527751287431</v>
+        <v>2.535076530612245</v>
       </c>
     </row>
     <row r="116" spans="1:43">
@@ -15318,10 +15885,10 @@
         <v>17.68202764976958</v>
       </c>
       <c r="AP116">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ116">
-        <v>33.05051897153193</v>
+        <v>2.858086365803273</v>
       </c>
     </row>
     <row r="117" spans="1:43">
@@ -15410,7 +15977,7 @@
         <v>0</v>
       </c>
       <c r="AP117">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ117">
         <v>0</v>
@@ -15541,10 +16108,10 @@
         <v>7.965250965250966</v>
       </c>
       <c r="AP118">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ118">
-        <v>14.88831956121676</v>
+        <v>1.287486686193583</v>
       </c>
     </row>
     <row r="119" spans="1:43">
@@ -15672,10 +16239,10 @@
         <v>7.796812749003984</v>
       </c>
       <c r="AP119">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ119">
-        <v>14.57348177383922</v>
+        <v>1.260260681412282</v>
       </c>
     </row>
     <row r="120" spans="1:43">
@@ -15760,14 +16327,35 @@
       <c r="AG120">
         <v>476.01</v>
       </c>
+      <c r="AH120">
+        <v>1.724025974025974</v>
+      </c>
+      <c r="AI120">
+        <v>0.1103896103896104</v>
+      </c>
+      <c r="AJ120">
+        <v>0</v>
+      </c>
+      <c r="AK120">
+        <v>0</v>
+      </c>
+      <c r="AL120">
+        <v>0</v>
+      </c>
+      <c r="AM120">
+        <v>1.006493506493507</v>
+      </c>
+      <c r="AN120">
+        <v>0</v>
+      </c>
       <c r="AO120">
-        <v>0</v>
+        <v>2.840909090909091</v>
       </c>
       <c r="AP120">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ120">
-        <v>0</v>
+        <v>0.4591986677115987</v>
       </c>
     </row>
     <row r="121" spans="1:43">
@@ -15895,10 +16483,10 @@
         <v>15.08</v>
       </c>
       <c r="AP121">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ121">
-        <v>28.18691588785047</v>
+        <v>2.4375</v>
       </c>
     </row>
     <row r="122" spans="1:43">
@@ -16026,10 +16614,10 @@
         <v>10.72641509433962</v>
       </c>
       <c r="AP122">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ122">
-        <v>20.04937400811145</v>
+        <v>1.733795543266103</v>
       </c>
     </row>
     <row r="123" spans="1:43">
@@ -16157,10 +16745,10 @@
         <v>8.672413793103448</v>
       </c>
       <c r="AP123">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ123">
-        <v>16.2101192394457</v>
+        <v>1.401791022592152</v>
       </c>
     </row>
     <row r="124" spans="1:43">
@@ -16267,7 +16855,7 @@
         <v>0</v>
       </c>
       <c r="AP124">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ124">
         <v>0</v>
@@ -16398,10 +16986,10 @@
         <v>11.1566265060241</v>
       </c>
       <c r="AP125">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ125">
-        <v>20.85350748789551</v>
+        <v>1.803334025758205</v>
       </c>
     </row>
     <row r="126" spans="1:43">
@@ -16508,7 +17096,7 @@
         <v>0</v>
       </c>
       <c r="AP126">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ126">
         <v>0</v>
@@ -16615,7 +17203,7 @@
         <v>0</v>
       </c>
       <c r="AP127">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ127">
         <v>0</v>
@@ -16746,10 +17334,10 @@
         <v>13.14423076923077</v>
       </c>
       <c r="AP128">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ128">
-        <v>24.568655643422</v>
+        <v>2.124606266578249</v>
       </c>
     </row>
     <row r="129" spans="1:43">
@@ -16877,10 +17465,10 @@
         <v>13.04347826086956</v>
       </c>
       <c r="AP129">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ129">
-        <v>24.38033319788704</v>
+        <v>2.10832083958021</v>
       </c>
     </row>
     <row r="130" spans="1:43">
@@ -17008,10 +17596,10 @@
         <v>13.64</v>
       </c>
       <c r="AP130">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ130">
-        <v>25.49532710280373</v>
+        <v>2.204741379310345</v>
       </c>
     </row>
     <row r="131" spans="1:43">
@@ -17139,10 +17727,10 @@
         <v>12.304</v>
       </c>
       <c r="AP131">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ131">
-        <v>22.99813084112149</v>
+        <v>1.988793103448276</v>
       </c>
     </row>
     <row r="132" spans="1:43">
@@ -17231,7 +17819,7 @@
         <v>0</v>
       </c>
       <c r="AP132">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ132">
         <v>0</v>
@@ -17337,14 +17925,35 @@
       <c r="AG133">
         <v>468.76</v>
       </c>
+      <c r="AH133">
+        <v>2.995967741935484</v>
+      </c>
+      <c r="AI133">
+        <v>2.209677419354839</v>
+      </c>
+      <c r="AJ133">
+        <v>0.2379032258064516</v>
+      </c>
+      <c r="AK133">
+        <v>1.354838709677419</v>
+      </c>
+      <c r="AL133">
+        <v>1.645161290322581</v>
+      </c>
+      <c r="AM133">
+        <v>2.217741935483871</v>
+      </c>
+      <c r="AN133">
+        <v>0.03629032258064516</v>
+      </c>
       <c r="AO133">
-        <v>0</v>
+        <v>10.69758064516129</v>
       </c>
       <c r="AP133">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ133">
-        <v>0</v>
+        <v>1.729134802558398</v>
       </c>
     </row>
     <row r="134" spans="1:43">
@@ -17451,7 +18060,7 @@
         <v>0</v>
       </c>
       <c r="AP134">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ134">
         <v>0</v>
@@ -17515,14 +18124,35 @@
       <c r="AG135">
         <v>375.72</v>
       </c>
+      <c r="AH135">
+        <v>1.704545454545455</v>
+      </c>
+      <c r="AI135">
+        <v>0.7662337662337663</v>
+      </c>
+      <c r="AJ135">
+        <v>0</v>
+      </c>
+      <c r="AK135">
+        <v>0</v>
+      </c>
+      <c r="AL135">
+        <v>2.266233766233766</v>
+      </c>
+      <c r="AM135">
+        <v>0.6298701298701299</v>
+      </c>
+      <c r="AN135">
+        <v>0.737012987012987</v>
+      </c>
       <c r="AO135">
-        <v>0</v>
+        <v>6.103896103896104</v>
       </c>
       <c r="AP135">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ135">
-        <v>0</v>
+        <v>0.9866211374832065</v>
       </c>
     </row>
     <row r="136" spans="1:43">
@@ -17650,10 +18280,10 @@
         <v>12.64453125</v>
       </c>
       <c r="AP136">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ136">
-        <v>23.63463785046729</v>
+        <v>2.043835870150862</v>
       </c>
     </row>
     <row r="137" spans="1:43">
@@ -17781,10 +18411,10 @@
         <v>10.98360655737705</v>
       </c>
       <c r="AP137">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ137">
-        <v>20.53010571472345</v>
+        <v>1.775367439231204</v>
       </c>
     </row>
     <row r="138" spans="1:43">
@@ -17825,7 +18455,7 @@
         <v>0</v>
       </c>
       <c r="AP138">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ138">
         <v>0</v>
@@ -17931,14 +18561,35 @@
       <c r="AG139">
         <v>447.45</v>
       </c>
+      <c r="AH139">
+        <v>2.051948051948052</v>
+      </c>
+      <c r="AI139">
+        <v>1.636363636363636</v>
+      </c>
+      <c r="AJ139">
+        <v>1.100649350649351</v>
+      </c>
+      <c r="AK139">
+        <v>1.376623376623377</v>
+      </c>
+      <c r="AL139">
+        <v>2.688311688311688</v>
+      </c>
+      <c r="AM139">
+        <v>1.5</v>
+      </c>
+      <c r="AN139">
+        <v>1.435064935064935</v>
+      </c>
       <c r="AO139">
-        <v>0</v>
+        <v>11.78896103896104</v>
       </c>
       <c r="AP139">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ139">
-        <v>0</v>
+        <v>1.905543271383789</v>
       </c>
     </row>
     <row r="140" spans="1:43">
@@ -18066,10 +18717,10 @@
         <v>10.80838323353293</v>
       </c>
       <c r="AP140">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ140">
-        <v>20.20258548323913</v>
+        <v>1.747044703696056</v>
       </c>
     </row>
     <row r="141" spans="1:43">
@@ -18197,10 +18848,10 @@
         <v>13.08487084870849</v>
       </c>
       <c r="AP141">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ141">
-        <v>24.45770252095044</v>
+        <v>2.115011451838656</v>
       </c>
     </row>
     <row r="142" spans="1:43">
@@ -18328,10 +18979,10 @@
         <v>9.475806451612904</v>
       </c>
       <c r="AP142">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ142">
-        <v>17.71178776002412</v>
+        <v>1.531649749721913</v>
       </c>
     </row>
     <row r="143" spans="1:43">
@@ -18459,10 +19110,10 @@
         <v>7.447368421052632</v>
       </c>
       <c r="AP143">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ143">
-        <v>13.92031480570585</v>
+        <v>1.20377722323049</v>
       </c>
     </row>
     <row r="144" spans="1:43">
@@ -18565,11 +19216,32 @@
       <c r="AG144">
         <v>446.17</v>
       </c>
+      <c r="AH144">
+        <v>0</v>
+      </c>
+      <c r="AI144">
+        <v>0</v>
+      </c>
+      <c r="AJ144">
+        <v>0</v>
+      </c>
+      <c r="AK144">
+        <v>0</v>
+      </c>
+      <c r="AL144">
+        <v>0</v>
+      </c>
+      <c r="AM144">
+        <v>0</v>
+      </c>
+      <c r="AN144">
+        <v>0</v>
+      </c>
       <c r="AO144">
         <v>0</v>
       </c>
       <c r="AP144">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ144">
         <v>0</v>
@@ -18700,10 +19372,10 @@
         <v>10.30434782608696</v>
       </c>
       <c r="AP145">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ145">
-        <v>19.26046322633076</v>
+        <v>1.665573463268366</v>
       </c>
     </row>
     <row r="146" spans="1:43">
@@ -18831,10 +19503,10 @@
         <v>12.50793650793651</v>
       </c>
       <c r="AP146">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ146">
-        <v>23.37932057558226</v>
+        <v>2.021756978653531</v>
       </c>
     </row>
     <row r="147" spans="1:43">
@@ -18941,7 +19613,7 @@
         <v>0</v>
       </c>
       <c r="AP147">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ147">
         <v>0</v>
@@ -19072,10 +19744,10 @@
         <v>6.24124513618677</v>
       </c>
       <c r="AP148">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ148">
-        <v>11.66587875922761</v>
+        <v>1.008821950892258</v>
       </c>
     </row>
     <row r="149" spans="1:43">
@@ -19203,10 +19875,10 @@
         <v>13.76223776223776</v>
       </c>
       <c r="AP149">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ149">
-        <v>25.72380890137899</v>
+        <v>2.224499638292742</v>
       </c>
     </row>
     <row r="150" spans="1:43">
@@ -19334,10 +20006,10 @@
         <v>13.73275862068965</v>
       </c>
       <c r="AP150">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ150">
-        <v>25.66870770222365</v>
+        <v>2.219734690844233</v>
       </c>
     </row>
     <row r="151" spans="1:43">
@@ -19398,14 +20070,35 @@
       <c r="AG151">
         <v>381.68</v>
       </c>
+      <c r="AH151">
+        <v>2.25974025974026</v>
+      </c>
+      <c r="AI151">
+        <v>1.834415584415584</v>
+      </c>
+      <c r="AJ151">
+        <v>1.457792207792208</v>
+      </c>
+      <c r="AK151">
+        <v>1.519480519480519</v>
+      </c>
+      <c r="AL151">
+        <v>2.425324675324675</v>
+      </c>
+      <c r="AM151">
+        <v>1.512987012987013</v>
+      </c>
+      <c r="AN151">
+        <v>1.402597402597403</v>
+      </c>
       <c r="AO151">
-        <v>0</v>
+        <v>12.41233766233766</v>
       </c>
       <c r="AP151">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ151">
-        <v>0</v>
+        <v>2.006304579041648</v>
       </c>
     </row>
     <row r="152" spans="1:43">
@@ -19533,10 +20226,10 @@
         <v>15.34108527131783</v>
       </c>
       <c r="AP152">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ152">
-        <v>28.67492574078099</v>
+        <v>2.479701283079391</v>
       </c>
     </row>
     <row r="153" spans="1:43">
@@ -19664,10 +20357,10 @@
         <v>10.58904109589041</v>
       </c>
       <c r="AP153">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ153">
-        <v>19.79260017923441</v>
+        <v>1.711590694378838</v>
       </c>
     </row>
     <row r="154" spans="1:43">
@@ -19795,10 +20488,10 @@
         <v>15.69191919191919</v>
       </c>
       <c r="AP154">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ154">
-        <v>29.33069007835363</v>
+        <v>2.53640935214211</v>
       </c>
     </row>
     <row r="155" spans="1:43">
@@ -19926,10 +20619,10 @@
         <v>16.38690476190476</v>
       </c>
       <c r="AP155">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ155">
-        <v>30.62972852692479</v>
+        <v>2.648745381773399</v>
       </c>
     </row>
     <row r="156" spans="1:43">
@@ -20057,10 +20750,10 @@
         <v>13.375</v>
       </c>
       <c r="AP156">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ156">
-        <v>25</v>
+        <v>2.161907327586207</v>
       </c>
     </row>
     <row r="157" spans="1:43">
@@ -20121,11 +20814,32 @@
       <c r="AG157">
         <v>391.58</v>
       </c>
+      <c r="AH157">
+        <v>0</v>
+      </c>
+      <c r="AI157">
+        <v>0</v>
+      </c>
+      <c r="AJ157">
+        <v>0</v>
+      </c>
+      <c r="AK157">
+        <v>0</v>
+      </c>
+      <c r="AL157">
+        <v>0</v>
+      </c>
+      <c r="AM157">
+        <v>0</v>
+      </c>
+      <c r="AN157">
+        <v>0</v>
+      </c>
       <c r="AO157">
         <v>0</v>
       </c>
       <c r="AP157">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ157">
         <v>0</v>
@@ -20256,10 +20970,10 @@
         <v>7.83399209486166</v>
       </c>
       <c r="AP158">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ158">
-        <v>14.64297587824609</v>
+        <v>1.266270273953932</v>
       </c>
     </row>
     <row r="159" spans="1:43">
@@ -20387,10 +21101,10 @@
         <v>11.96062992125984</v>
       </c>
       <c r="AP159">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ159">
-        <v>22.35631760983148</v>
+        <v>1.933291474341569</v>
       </c>
     </row>
     <row r="160" spans="1:43">
@@ -20493,14 +21207,35 @@
       <c r="AG160">
         <v>407.96</v>
       </c>
+      <c r="AH160">
+        <v>2.220779220779221</v>
+      </c>
+      <c r="AI160">
+        <v>1.564935064935065</v>
+      </c>
+      <c r="AJ160">
+        <v>1.444805194805195</v>
+      </c>
+      <c r="AK160">
+        <v>0.6655844155844156</v>
+      </c>
+      <c r="AL160">
+        <v>2.532467532467532</v>
+      </c>
+      <c r="AM160">
+        <v>1.5</v>
+      </c>
+      <c r="AN160">
+        <v>1.392857142857143</v>
+      </c>
       <c r="AO160">
-        <v>0</v>
+        <v>11.32142857142857</v>
       </c>
       <c r="AP160">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ160">
-        <v>0</v>
+        <v>1.829972290640394</v>
       </c>
     </row>
     <row r="161" spans="1:43">
@@ -20628,10 +21363,10 @@
         <v>12.77083333333333</v>
       </c>
       <c r="AP161">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ161">
-        <v>23.87071651090343</v>
+        <v>2.064251077586207</v>
       </c>
     </row>
     <row r="162" spans="1:43">
@@ -20759,10 +21494,10 @@
         <v>9.203065134099615</v>
       </c>
       <c r="AP162">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ162">
-        <v>17.20199090485909</v>
+        <v>1.487564407451446</v>
       </c>
     </row>
     <row r="163" spans="1:43">
@@ -20890,10 +21625,10 @@
         <v>11.14285714285714</v>
       </c>
       <c r="AP163">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ163">
-        <v>20.82777036048064</v>
+        <v>1.801108374384236</v>
       </c>
     </row>
     <row r="164" spans="1:43">
@@ -21021,10 +21756,10 @@
         <v>13.04819277108434</v>
       </c>
       <c r="AP164">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ164">
-        <v>24.38914536651279</v>
+        <v>2.109082883257167</v>
       </c>
     </row>
     <row r="165" spans="1:43">
@@ -21113,7 +21848,7 @@
         <v>0</v>
       </c>
       <c r="AP165">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ165">
         <v>0</v>
@@ -21223,7 +21958,7 @@
         <v>0</v>
       </c>
       <c r="AP166">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ166">
         <v>0</v>
@@ -21333,7 +22068,7 @@
         <v>0</v>
       </c>
       <c r="AP167">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ167">
         <v>0</v>
@@ -21446,10 +22181,10 @@
         <v>7.274131274131274</v>
       </c>
       <c r="AP168">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ168">
-        <v>13.59650705445098</v>
+        <v>1.175775529223805</v>
       </c>
     </row>
     <row r="169" spans="1:43">
@@ -21556,7 +22291,7 @@
         <v>0</v>
       </c>
       <c r="AP169">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ169">
         <v>0</v>
@@ -21687,10 +22422,10 @@
         <v>14.84684684684685</v>
       </c>
       <c r="AP170">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ170">
-        <v>27.75111560158289</v>
+        <v>2.399813606710159</v>
       </c>
     </row>
     <row r="171" spans="1:43">
@@ -21818,10 +22553,10 @@
         <v>9.121951219512194</v>
       </c>
       <c r="AP171">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ171">
-        <v>17.05037611123775</v>
+        <v>1.474453322119428</v>
       </c>
     </row>
     <row r="172" spans="1:43">
@@ -21925,10 +22660,10 @@
         <v>10.92857142857143</v>
       </c>
       <c r="AP172">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ172">
-        <v>20.42723631508678</v>
+        <v>1.766471674876847</v>
       </c>
     </row>
     <row r="173" spans="1:43">
@@ -22031,14 +22766,35 @@
       <c r="AG173">
         <v>483.25</v>
       </c>
+      <c r="AH173">
+        <v>1.463114754098361</v>
+      </c>
+      <c r="AI173">
+        <v>0.5491803278688525</v>
+      </c>
+      <c r="AJ173">
+        <v>0.2049180327868853</v>
+      </c>
+      <c r="AK173">
+        <v>0.2131147540983606</v>
+      </c>
+      <c r="AL173">
+        <v>2.14344262295082</v>
+      </c>
+      <c r="AM173">
+        <v>0.7704918032786885</v>
+      </c>
+      <c r="AN173">
+        <v>0.3278688524590164</v>
+      </c>
       <c r="AO173">
-        <v>0</v>
+        <v>5.672131147540984</v>
       </c>
       <c r="AP173">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ173">
-        <v>0</v>
+        <v>0.9168315432447711</v>
       </c>
     </row>
     <row r="174" spans="1:43">
@@ -22166,10 +22922,10 @@
         <v>14.91803278688525</v>
       </c>
       <c r="AP174">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ174">
-        <v>27.88417343343037</v>
+        <v>2.41131995477671</v>
       </c>
     </row>
     <row r="175" spans="1:43">
@@ -22297,10 +23053,10 @@
         <v>5.063157894736842</v>
       </c>
       <c r="AP175">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ175">
-        <v>9.463846532218398</v>
+        <v>0.8183983666061706</v>
       </c>
     </row>
     <row r="176" spans="1:43">
@@ -22379,14 +23135,35 @@
       <c r="Y176">
         <v>105422</v>
       </c>
+      <c r="AH176">
+        <v>1.659090909090909</v>
+      </c>
+      <c r="AI176">
+        <v>0.7012987012987013</v>
+      </c>
+      <c r="AJ176">
+        <v>0.4383116883116883</v>
+      </c>
+      <c r="AK176">
+        <v>0.6461038961038961</v>
+      </c>
+      <c r="AL176">
+        <v>1.980519480519481</v>
+      </c>
+      <c r="AM176">
+        <v>0.8636363636363636</v>
+      </c>
+      <c r="AN176">
+        <v>0.3766233766233766</v>
+      </c>
       <c r="AO176">
-        <v>0</v>
+        <v>6.665584415584415</v>
       </c>
       <c r="AP176">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ176">
-        <v>0</v>
+        <v>1.077411274070757</v>
       </c>
     </row>
     <row r="177" spans="1:43">
@@ -22451,7 +23228,7 @@
         <v>0</v>
       </c>
       <c r="AP177">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ177">
         <v>0</v>
@@ -22582,10 +23359,10 @@
         <v>8.533333333333333</v>
       </c>
       <c r="AP178">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ178">
-        <v>15.95015576323988</v>
+        <v>1.379310344827586</v>
       </c>
     </row>
     <row r="179" spans="1:43">
@@ -22713,10 +23490,10 @@
         <v>53.5</v>
       </c>
       <c r="AP179">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ179">
-        <v>100</v>
+        <v>8.647629310344827</v>
       </c>
     </row>
     <row r="180" spans="1:43">
@@ -22838,10 +23615,10 @@
         <v>8.675000000000001</v>
       </c>
       <c r="AP180">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ180">
-        <v>16.21495327102804</v>
+        <v>1.402209051724138</v>
       </c>
     </row>
     <row r="181" spans="1:43">
@@ -22969,10 +23746,10 @@
         <v>12.97810218978102</v>
       </c>
       <c r="AP181">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ181">
-        <v>24.25813493417014</v>
+        <v>2.097753586710295</v>
       </c>
     </row>
     <row r="182" spans="1:43">
@@ -23100,10 +23877,10 @@
         <v>4.75609756097561</v>
       </c>
       <c r="AP182">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ182">
-        <v>8.889901983131981</v>
+        <v>0.7687657695542474</v>
       </c>
     </row>
     <row r="183" spans="1:43">
@@ -23222,10 +23999,10 @@
         <v>18.37735849056604</v>
       </c>
       <c r="AP183">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ183">
-        <v>34.35020278610475</v>
+        <v>2.970478204294079</v>
       </c>
     </row>
     <row r="184" spans="1:43">
@@ -23353,10 +24130,10 @@
         <v>11.23381294964029</v>
       </c>
       <c r="AP184">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ184">
-        <v>20.99778121428091</v>
+        <v>1.815810282808236</v>
       </c>
     </row>
     <row r="185" spans="1:43">
@@ -23484,10 +24261,10 @@
         <v>8.148014440433213</v>
       </c>
       <c r="AP185">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ185">
-        <v>15.22993353352003</v>
+        <v>1.317028196190713</v>
       </c>
     </row>
     <row r="186" spans="1:43">
@@ -23615,10 +24392,10 @@
         <v>14.44736842105263</v>
       </c>
       <c r="AP186">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ186">
-        <v>27.00442695523856</v>
+        <v>2.33524274047187</v>
       </c>
     </row>
     <row r="187" spans="1:43">
@@ -23746,10 +24523,10 @@
         <v>14.60130718954248</v>
       </c>
       <c r="AP187">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ187">
-        <v>27.29216297110744</v>
+        <v>2.360125084516565</v>
       </c>
     </row>
     <row r="188" spans="1:43">
@@ -23877,10 +24654,10 @@
         <v>4.562937062937063</v>
       </c>
       <c r="AP188">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ188">
-        <v>8.528854323246847</v>
+        <v>0.7375437062937064</v>
       </c>
     </row>
     <row r="189" spans="1:43">
@@ -23983,14 +24760,35 @@
       <c r="AG189">
         <v>750.02</v>
       </c>
+      <c r="AH189">
+        <v>1.278625954198473</v>
+      </c>
+      <c r="AI189">
+        <v>1.67175572519084</v>
+      </c>
+      <c r="AJ189">
+        <v>0</v>
+      </c>
+      <c r="AK189">
+        <v>0.3091603053435115</v>
+      </c>
+      <c r="AL189">
+        <v>2.854961832061069</v>
+      </c>
+      <c r="AM189">
+        <v>1.812977099236641</v>
+      </c>
+      <c r="AN189">
+        <v>0.3702290076335878</v>
+      </c>
       <c r="AO189">
-        <v>0</v>
+        <v>8.297709923664122</v>
       </c>
       <c r="AP189">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ189">
-        <v>0</v>
+        <v>1.341224664385365</v>
       </c>
     </row>
     <row r="190" spans="1:43">
@@ -24076,10 +24874,10 @@
         <v>13.3046357615894</v>
       </c>
       <c r="AP190">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ190">
-        <v>24.86847805904561</v>
+        <v>2.150533797670701</v>
       </c>
     </row>
     <row r="191" spans="1:43">
@@ -24195,10 +24993,10 @@
         <v>1.444444444444445</v>
       </c>
       <c r="AP191">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ191">
-        <v>2.699896157840084</v>
+        <v>0.2334770114942529</v>
       </c>
     </row>
     <row r="192" spans="1:43">
@@ -24326,10 +25124,10 @@
         <v>8.545454545454545</v>
       </c>
       <c r="AP192">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ192">
-        <v>15.97281223449448</v>
+        <v>1.381269592476489</v>
       </c>
     </row>
     <row r="193" spans="1:43">
@@ -24457,10 +25255,10 @@
         <v>7.75</v>
       </c>
       <c r="AP193">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ193">
-        <v>14.48598130841122</v>
+        <v>1.252693965517241</v>
       </c>
     </row>
     <row r="194" spans="1:43">
@@ -24588,10 +25386,10 @@
         <v>3.208333333333333</v>
       </c>
       <c r="AP194">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ194">
-        <v>5.996884735202491</v>
+        <v>0.5185883620689655</v>
       </c>
     </row>
     <row r="195" spans="1:43">
@@ -24719,10 +25517,10 @@
         <v>11.7</v>
       </c>
       <c r="AP195">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ195">
-        <v>21.86915887850467</v>
+        <v>1.891163793103448</v>
       </c>
     </row>
     <row r="196" spans="1:43">
@@ -24850,10 +25648,10 @@
         <v>8.892430278884463</v>
       </c>
       <c r="AP196">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ196">
-        <v>16.62136500726068</v>
+        <v>1.437354032147273</v>
       </c>
     </row>
     <row r="197" spans="1:43">
@@ -24981,10 +25779,10 @@
         <v>13.24864864864865</v>
       </c>
       <c r="AP197">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ197">
-        <v>24.76382924981056</v>
+        <v>2.141484156570364</v>
       </c>
     </row>
     <row r="198" spans="1:43">
@@ -25112,10 +25910,10 @@
         <v>7.628205128205129</v>
       </c>
       <c r="AP198">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ198">
-        <v>14.25832734243949</v>
+        <v>1.233007294429708</v>
       </c>
     </row>
     <row r="199" spans="1:43">
@@ -25243,10 +26041,10 @@
         <v>9.891891891891893</v>
       </c>
       <c r="AP199">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ199">
-        <v>18.48951755493812</v>
+        <v>1.598904939422181</v>
       </c>
     </row>
     <row r="200" spans="1:43">
@@ -25349,14 +26147,35 @@
       <c r="AG200">
         <v>460.2</v>
       </c>
+      <c r="AH200">
+        <v>0.7077922077922078</v>
+      </c>
+      <c r="AI200">
+        <v>0.6948051948051948</v>
+      </c>
+      <c r="AJ200">
+        <v>0.1331168831168831</v>
+      </c>
+      <c r="AK200">
+        <v>1.415584415584416</v>
+      </c>
+      <c r="AL200">
+        <v>0</v>
+      </c>
+      <c r="AM200">
+        <v>0.6883116883116883</v>
+      </c>
+      <c r="AN200">
+        <v>0</v>
+      </c>
       <c r="AO200">
-        <v>0</v>
+        <v>3.63961038961039</v>
       </c>
       <c r="AP200">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ200">
-        <v>0</v>
+        <v>0.588299093148231</v>
       </c>
     </row>
     <row r="201" spans="1:43">
@@ -25438,14 +26257,35 @@
       <c r="AG201">
         <v>412.86</v>
       </c>
+      <c r="AH201">
+        <v>1.616883116883117</v>
+      </c>
+      <c r="AI201">
+        <v>1.165584415584416</v>
+      </c>
+      <c r="AJ201">
+        <v>0</v>
+      </c>
+      <c r="AK201">
+        <v>0.7987012987012987</v>
+      </c>
+      <c r="AL201">
+        <v>1.948051948051948</v>
+      </c>
+      <c r="AM201">
+        <v>1.006493506493507</v>
+      </c>
+      <c r="AN201">
+        <v>0.7987012987012987</v>
+      </c>
       <c r="AO201">
-        <v>0</v>
+        <v>7.334415584415584</v>
       </c>
       <c r="AP201">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ201">
-        <v>0</v>
+        <v>1.185519760412002</v>
       </c>
     </row>
     <row r="202" spans="1:43">
@@ -25573,10 +26413,10 @@
         <v>16.37234042553191</v>
       </c>
       <c r="AP202">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ202">
-        <v>30.60250546828395</v>
+        <v>2.646391232575202</v>
       </c>
     </row>
     <row r="203" spans="1:43">
@@ -25704,10 +26544,10 @@
         <v>11.41176470588235</v>
       </c>
       <c r="AP203">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ203">
-        <v>21.33040131940626</v>
+        <v>1.844574036511156</v>
       </c>
     </row>
     <row r="204" spans="1:43">
@@ -25835,10 +26675,10 @@
         <v>9.179487179487181</v>
       </c>
       <c r="AP204">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ204">
-        <v>17.15791996165828</v>
+        <v>1.483753315649868</v>
       </c>
     </row>
     <row r="205" spans="1:43">
@@ -25966,10 +26806,10 @@
         <v>11.90940766550523</v>
       </c>
       <c r="AP205">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ205">
-        <v>22.2605750757107</v>
+        <v>1.925012014898474</v>
       </c>
     </row>
     <row r="206" spans="1:43">
@@ -26097,10 +26937,10 @@
         <v>12.20408163265306</v>
       </c>
       <c r="AP206">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ206">
-        <v>22.81136753766927</v>
+        <v>1.972642505277973</v>
       </c>
     </row>
     <row r="207" spans="1:43">
@@ -26228,10 +27068,10 @@
         <v>5.787755102040816</v>
       </c>
       <c r="AP207">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ207">
-        <v>10.81823383559031</v>
+        <v>0.9355207600281492</v>
       </c>
     </row>
     <row r="208" spans="1:43">
@@ -26359,10 +27199,10 @@
         <v>15.26573426573426</v>
       </c>
       <c r="AP208">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ208">
-        <v>28.53408273969022</v>
+        <v>2.467521702435496</v>
       </c>
     </row>
     <row r="209" spans="1:43">
@@ -26465,14 +27305,35 @@
       <c r="AG209">
         <v>442.33</v>
       </c>
+      <c r="AH209">
+        <v>53</v>
+      </c>
+      <c r="AI209">
+        <v>103.3333333333333</v>
+      </c>
+      <c r="AJ209">
+        <v>51.66666666666666</v>
+      </c>
+      <c r="AK209">
+        <v>57</v>
+      </c>
+      <c r="AL209">
+        <v>198.6666666666667</v>
+      </c>
+      <c r="AM209">
+        <v>103.3333333333333</v>
+      </c>
+      <c r="AN209">
+        <v>51.66666666666666</v>
+      </c>
       <c r="AO209">
-        <v>0</v>
+        <v>618.6666666666666</v>
       </c>
       <c r="AP209">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ209">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="210" spans="1:43">
@@ -26594,10 +27455,10 @@
         <v>15.90445859872611</v>
       </c>
       <c r="AP210">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ210">
-        <v>29.7279599976189</v>
+        <v>2.570763782121678</v>
       </c>
     </row>
     <row r="211" spans="1:43">
@@ -26725,10 +27586,10 @@
         <v>9.642857142857142</v>
       </c>
       <c r="AP211">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ211">
-        <v>18.02403204272363</v>
+        <v>1.558651477832512</v>
       </c>
     </row>
     <row r="212" spans="1:43">
@@ -26835,7 +27696,7 @@
         <v>0</v>
       </c>
       <c r="AP212">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ212">
         <v>0</v>
@@ -26903,7 +27764,7 @@
         <v>0</v>
       </c>
       <c r="AP213">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ213">
         <v>0</v>
@@ -27034,10 +27895,10 @@
         <v>11.01470588235294</v>
       </c>
       <c r="AP214">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ214">
-        <v>20.58823529411765</v>
+        <v>1.780394269776877</v>
       </c>
     </row>
     <row r="215" spans="1:43">
@@ -27165,10 +28026,10 @@
         <v>8.617647058823529</v>
       </c>
       <c r="AP215">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ215">
-        <v>16.10775151181968</v>
+        <v>1.392938640973631</v>
       </c>
     </row>
     <row r="216" spans="1:43">
@@ -27296,10 +28157,10 @@
         <v>14.08088235294118</v>
       </c>
       <c r="AP216">
-        <v>1.869158878504673</v>
+        <v>0.1616379310344828</v>
       </c>
       <c r="AQ216">
-        <v>26.31940626717977</v>
+        <v>2.276004690669371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>